<commit_message>
Updated the rest of the test files
</commit_message>
<xml_diff>
--- a/test_files/perturbation_tests/to_be_reformatted/seaver_L-curve/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_no-graph_test22_output.xlsx
+++ b/test_files/perturbation_tests/to_be_reformatted/seaver_L-curve/4-genes_6-edges_artificial-data_Sigmoidal_estimation_fixb-1_fixP-1_no-graph_test22_output.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="40">
   <si>
     <t>CIN5</t>
   </si>
@@ -2480,7 +2480,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="C1" sqref="C1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2488,27 +2488,15 @@
     <col min="1" max="1" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2516,7 +2504,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2524,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2532,7 +2520,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2540,7 +2528,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2548,7 +2536,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2556,7 +2544,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2564,7 +2552,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -2572,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2580,7 +2568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2588,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2596,7 +2584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2604,7 +2592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -2621,7 +2609,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2632,7 +2620,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>